<commit_message>
3.3.1.1 --> 3.4.0 update land/CApULAbIFM (set to value from U.S. file)
</commit_message>
<xml_diff>
--- a/InputData/land/CApULAbIFM/CO2 Abated per Unit Land Area by Impr For Mgmt.xlsx
+++ b/InputData/land/CApULAbIFM/CO2 Abated per Unit Land Area by Impr For Mgmt.xlsx
@@ -1,22 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dobrien\Dropbox (Energy Innovation)\Desktop\Models\E.U. Models\eps-eu\InputData\land\CApULAbIFM\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{846746B8-F908-4769-9B52-96FEC312D293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="315" yWindow="315" windowWidth="18825" windowHeight="6555"/>
+    <workbookView xWindow="1480" yWindow="1480" windowWidth="16420" windowHeight="9350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
-    <sheet name="Calculations" sheetId="4" r:id="rId2"/>
-    <sheet name="CApULAbIFM" sheetId="3" r:id="rId3"/>
+    <sheet name="CApULAbIFM" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>CApULAbIFM CO2 Abated per Unit Land Area by Improved Forest Management</t>
   </si>
@@ -30,43 +48,13 @@
     <t>Per Acre</t>
   </si>
   <si>
-    <t>Increased Annual CO2 Sequestration Achievable by Improved Management Practices per Acre</t>
-  </si>
-  <si>
-    <t>tons CO2 / acre / yr</t>
-  </si>
-  <si>
-    <t>Low Estimate</t>
-  </si>
-  <si>
-    <t>High Estimate</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>g CO2 / acre / yr</t>
-  </si>
-  <si>
-    <t>Average, converted to grams CO2</t>
-  </si>
-  <si>
-    <t>U.S. EPA</t>
-  </si>
-  <si>
-    <t>Greenhouse Gas Mitigation Potential in U.S. Forestry and Agriculture</t>
-  </si>
-  <si>
-    <t>http://www.epa.gov/climate/climatechange/Downloads/ccs/ghg_mitigation_forestry_ag_2005.pdf</t>
-  </si>
-  <si>
-    <t>Page 2-3, Table 2-1</t>
+    <t>Consultation with American Forest Foundation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -135,6 +123,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -182,7 +173,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -215,9 +206,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -250,6 +258,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -425,141 +450,64 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
-      <c r="B4" s="4">
-        <v>2005</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="4"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
-      <c r="B6" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="5"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:2" ht="14.45" x14ac:dyDescent="0.35"/>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="19" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2.1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>3.1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <f>AVERAGE(A2:A3)</f>
-        <v>2.6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <f>A4*10^6</f>
-        <v>2600000</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="1" max="1" width="15.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -572,8 +520,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="3">
-        <f>Calculations!A6</f>
-        <v>2600000</v>
+        <v>1500000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Uploading Agora/EI land and trans data files
</commit_message>
<xml_diff>
--- a/InputData/land/CApULAbIFM/CO2 Abated per Unit Land Area by Impr For Mgmt.xlsx
+++ b/InputData/land/CApULAbIFM/CO2 Abated per Unit Land Area by Impr For Mgmt.xlsx
@@ -1,23 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\land\CApULAbIFM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://energyinnovation.sharepoint.com/sites/EUEPSModeling/Shared Documents/InputData_EI+Agora/land/CApULAbIFM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF08A53-F280-4704-83EC-0E3DACD573C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="13_ncr:1_{3EF08A53-F280-4704-83EC-0E3DACD573C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C91ADF6-5A35-4292-B74B-BCB7992215E1}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
-    <sheet name="CApULAbIFM" sheetId="3" r:id="rId2"/>
+    <sheet name="Data" sheetId="4" r:id="rId2"/>
+    <sheet name="CApULAbIFM" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -25,6 +29,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>CApULAbIFM CO2 Abated per Unit Land Area by Improved Forest Management</t>
   </si>
@@ -40,20 +46,65 @@
     <t>Source:</t>
   </si>
   <si>
+    <t>CO2 per land unit: forest management</t>
+  </si>
+  <si>
+    <t>Nature4Climate</t>
+  </si>
+  <si>
+    <t>US Carbon Mapper</t>
+  </si>
+  <si>
+    <t>https://nature4climate.org/nature-in-action/ncs-world-atlas/</t>
+  </si>
+  <si>
+    <t>Data underlying the online mapper send by Chris Zganjar upon request March 2023</t>
+  </si>
+  <si>
+    <t>Total EU Forest Acreage</t>
+  </si>
+  <si>
+    <t>Eurostat</t>
+  </si>
+  <si>
+    <t>Area of wooded land</t>
+  </si>
+  <si>
+    <t>https://ec.europa.eu/eurostat/databrowser/view/FOR_AREA_EFA__custom_672302/bookmark/table?lang=en&amp;bookmarkId=2b089c56-a550-4f87-943e-0989dacf605a</t>
+  </si>
+  <si>
+    <t>EU Forest Acreage</t>
+  </si>
+  <si>
+    <t>thousand hectares</t>
+  </si>
+  <si>
+    <t>acres</t>
+  </si>
+  <si>
+    <t>Per Acre</t>
+  </si>
+  <si>
     <t>CO2 Abated (g)</t>
   </si>
   <si>
-    <t>Per Acre</t>
-  </si>
-  <si>
-    <t>consultation with American Forest Foundation</t>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>TgCO2e/year</t>
+  </si>
+  <si>
+    <t>Improved Forest Management</t>
+  </si>
+  <si>
+    <t>Total abatement potential</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -69,13 +120,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -90,14 +161,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -116,9 +195,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -156,9 +235,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -191,26 +270,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -243,26 +305,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -436,67 +481,462 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="76.1796875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B5" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-    </row>
-    <row r="6" spans="1:2" ht="14.45" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B7" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B9" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B11" s="5">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B13" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8382EF59-A10D-4ACA-A2F1-587B3F39B01B}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.26953125" customWidth="1"/>
+    <col min="2" max="2" width="28.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="7"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>159497</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <f>A2*1000*2.471</f>
+        <v>394117087</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7">
+        <v>59.15</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="1" max="1" width="15.1796875" customWidth="1"/>
+    <col min="2" max="2" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" s="2" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="B2" s="3">
-        <f>1.5*10^6</f>
-        <v>1500000</v>
+        <f>(Data!C7*10^12)/Data!A3</f>
+        <v>150082.30282591123</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A08BDF573E2FFD46A5F05DED9AF68025" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f85c0eb68479ad8b8987805fd5b8836b">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00484652-42e1-479e-92f4-fb0efddcdf60" xmlns:ns3="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f7dbc72841229da9eaa30ebb1456cd70" ns2:_="" ns3:_="">
+    <xsd:import namespace="00484652-42e1-479e-92f4-fb0efddcdf60"/>
+    <xsd:import namespace="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="00484652-42e1-479e-92f4-fb0efddcdf60" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="10" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="12" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="eca5b831-c3dc-41cf-bd85-218b82cecb21" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="14" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="15" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="16" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="17" nillable="true" ma:displayName="Location" ma:indexed="true" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="18" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="TaxCatchAll" ma:index="13" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{c5b79d03-3bfd-4c46-9947-056a2403f6c9}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithUsers" ma:index="19" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="20" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5D857B3-7968-4F00-B6D5-7266C82B9E82}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
+    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17EA0462-F3C4-4FF4-946E-B2DEAE0AF014}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{093B51F1-6518-4D31-807F-B95E3F953940}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
+    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>